<commit_message>
Ajuste VIN y consultas BD
</commit_message>
<xml_diff>
--- a/Backend/data/Datos_Dummy_Vehiculos.xlsx
+++ b/Backend/data/Datos_Dummy_Vehiculos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\ProyectoConsultasEnLinea\Backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juand\Desktop\ProyectoConsultasEnLinea\Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19647E32-EFB9-46EA-B3CE-E5D14A3D41EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45970646-29E1-4E29-AEA3-A7DF79B2FB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="267">
   <si>
     <t>Numero de placa</t>
   </si>
@@ -523,6 +523,309 @@
   </si>
   <si>
     <t>ABC123</t>
+  </si>
+  <si>
+    <t>1HGCM82633A123456</t>
+  </si>
+  <si>
+    <t>JH4KA8260MC012345</t>
+  </si>
+  <si>
+    <t>1FTSW21R08ED56789</t>
+  </si>
+  <si>
+    <t>4T1BG22KXWU123456</t>
+  </si>
+  <si>
+    <t>2HGFG12856H654321</t>
+  </si>
+  <si>
+    <t>1J4GL48KX7W543210</t>
+  </si>
+  <si>
+    <t>1N4AL11D75C123456</t>
+  </si>
+  <si>
+    <t>2T2BZMCA2GC123456</t>
+  </si>
+  <si>
+    <t>5N1AT2MV5HC789012</t>
+  </si>
+  <si>
+    <t>JHMFA16586S012345</t>
+  </si>
+  <si>
+    <t>1HGCM66586A654321</t>
+  </si>
+  <si>
+    <t>4S4BP61C667789012</t>
+  </si>
+  <si>
+    <t>1C4NJPFA8CD123456</t>
+  </si>
+  <si>
+    <t>5XYKTDA26CG654321</t>
+  </si>
+  <si>
+    <t>1FMEU15N1SLC12345</t>
+  </si>
+  <si>
+    <t>3C4PDCBG0FT654321</t>
+  </si>
+  <si>
+    <t>1G1JC1244VJ123456</t>
+  </si>
+  <si>
+    <t>2G4WB52K8X1234567</t>
+  </si>
+  <si>
+    <t>2HGFA16578H654321</t>
+  </si>
+  <si>
+    <t>1HGEJ8240WL123456</t>
+  </si>
+  <si>
+    <t>JTHBE1BL5D5001234</t>
+  </si>
+  <si>
+    <t>1FTEX1C85AF123456</t>
+  </si>
+  <si>
+    <t>1C6RR7MT4FS654321</t>
+  </si>
+  <si>
+    <t>1FTFW1ET2EFB12345</t>
+  </si>
+  <si>
+    <t>3FAHP08148R654321</t>
+  </si>
+  <si>
+    <t>5J6RE4H56BL123456</t>
+  </si>
+  <si>
+    <t>1HGCP26798A123456</t>
+  </si>
+  <si>
+    <t>JTLKE50E591654321</t>
+  </si>
+  <si>
+    <t>1G4HR52KXWH123456</t>
+  </si>
+  <si>
+    <t>1FMRU1763VLA12345</t>
+  </si>
+  <si>
+    <t>JHMEG8650PS654321</t>
+  </si>
+  <si>
+    <t>JN8AZ1MU1AW123456</t>
+  </si>
+  <si>
+    <t>1FTNW21PX7EC12345</t>
+  </si>
+  <si>
+    <t>2LMPJ8LR8KBL12345</t>
+  </si>
+  <si>
+    <t>1FADP3F24EL123456</t>
+  </si>
+  <si>
+    <t>4S3BMBC69H1254321</t>
+  </si>
+  <si>
+    <t>1FTRX18L7YKC12345</t>
+  </si>
+  <si>
+    <t>1HGFA16527L654321</t>
+  </si>
+  <si>
+    <t>3FA6P0HR5DR123456</t>
+  </si>
+  <si>
+    <t>1HGCP36759A123456</t>
+  </si>
+  <si>
+    <t>JN8DR09Y82W654321</t>
+  </si>
+  <si>
+    <t>3VWDP7AJ4DM123456</t>
+  </si>
+  <si>
+    <t>5J6YH28696L123456</t>
+  </si>
+  <si>
+    <t>5NPEC4AC6BH654321</t>
+  </si>
+  <si>
+    <t>JNKCA21D5VT123456</t>
+  </si>
+  <si>
+    <t>2HGFG4A55DH654321</t>
+  </si>
+  <si>
+    <t>1C3CCCAB3FN123456</t>
+  </si>
+  <si>
+    <t>1GNDT13S692654321</t>
+  </si>
+  <si>
+    <t>3CZRU5H36GM123456</t>
+  </si>
+  <si>
+    <t>JN1CV6EK6HM654321</t>
+  </si>
+  <si>
+    <t>2HKRM4H56DH123456</t>
+  </si>
+  <si>
+    <t>3FADP4EJ0FM123456</t>
+  </si>
+  <si>
+    <t>5YJSA1H26EFP67890</t>
+  </si>
+  <si>
+    <t>1G1ZD5STXJF654321</t>
+  </si>
+  <si>
+    <t>1N6BA0CJ4FN123456</t>
+  </si>
+  <si>
+    <t>WBA3A9C57EF456789</t>
+  </si>
+  <si>
+    <t>1FTEX1CM4FKE12345</t>
+  </si>
+  <si>
+    <t>JHMGE8H56DC123456</t>
+  </si>
+  <si>
+    <t>2HGFC2F59HH654321</t>
+  </si>
+  <si>
+    <t>3VWLL7AJ7EM123456</t>
+  </si>
+  <si>
+    <t>5TDZK3EH0FS987654</t>
+  </si>
+  <si>
+    <t>2G1WB58K489123456</t>
+  </si>
+  <si>
+    <t>1GKS2BKC6GR123456</t>
+  </si>
+  <si>
+    <t>JN8AS5MT9CW987654</t>
+  </si>
+  <si>
+    <t>KMHCT4AE6HU123456</t>
+  </si>
+  <si>
+    <t>1D7RV1CP1AS654321</t>
+  </si>
+  <si>
+    <t>3GTU2NEC1EG123456</t>
+  </si>
+  <si>
+    <t>1FTFW1EF3EK456789</t>
+  </si>
+  <si>
+    <t>2C4RDGBG3FR123456</t>
+  </si>
+  <si>
+    <t>5XYPGDA35GG654321</t>
+  </si>
+  <si>
+    <t>1FAHP3FN1AW654321</t>
+  </si>
+  <si>
+    <t>5FNYF4H99BB123456</t>
+  </si>
+  <si>
+    <t>JA32U2FU6AU987654</t>
+  </si>
+  <si>
+    <t>3N1BC1AP8CL123456</t>
+  </si>
+  <si>
+    <t>5XXGN4A76EG123456</t>
+  </si>
+  <si>
+    <t>KM8SRDHF9EU654321</t>
+  </si>
+  <si>
+    <t>3VW517AT9DM456789</t>
+  </si>
+  <si>
+    <t>JTHBK262875123456</t>
+  </si>
+  <si>
+    <t>1HGEJ622XWL654321</t>
+  </si>
+  <si>
+    <t>2C3CCARG6FH123456</t>
+  </si>
+  <si>
+    <t>KM8K53A14JU123456</t>
+  </si>
+  <si>
+    <t>1C4PJMDS5GW123456</t>
+  </si>
+  <si>
+    <t>JN8AF5MR5ET654321</t>
+  </si>
+  <si>
+    <t>5TFAW5F12DX987654</t>
+  </si>
+  <si>
+    <t>4T4BF3EK9BR654321</t>
+  </si>
+  <si>
+    <t>3C6UR5FL1FG123456</t>
+  </si>
+  <si>
+    <t>1GCGC24R1ES654321</t>
+  </si>
+  <si>
+    <t>1GTW7AFG6G1212345</t>
+  </si>
+  <si>
+    <t>5FRYD3H29GB654321</t>
+  </si>
+  <si>
+    <t>5TFHW5F17GX123456</t>
+  </si>
+  <si>
+    <t>JTEBU5JR3E5678901</t>
+  </si>
+  <si>
+    <t>3FA6P0LU5HR654321</t>
+  </si>
+  <si>
+    <t>1GCGK29J1LE123456</t>
+  </si>
+  <si>
+    <t>1GNER13DXYJ654321</t>
+  </si>
+  <si>
+    <t>JHMCM56457S123456</t>
+  </si>
+  <si>
+    <t>4T1BE32K33U123456</t>
+  </si>
+  <si>
+    <t>2G1WT57K391234567</t>
+  </si>
+  <si>
+    <t>5J8TB4H36HL654321</t>
+  </si>
+  <si>
+    <t>JN8AZ2KR6HT654321</t>
+  </si>
+  <si>
+    <t>KMHCM3ACXBU123456</t>
+  </si>
+  <si>
+    <t>1HGCR2F32EA987654</t>
   </si>
 </sst>
 </file>
@@ -850,47 +1153,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H98" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="28" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="25.7265625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="45.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1294,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1028,8 +1331,8 @@
       <c r="L2">
         <v>123456</v>
       </c>
-      <c r="M2">
-        <v>123456</v>
+      <c r="M2" t="s">
+        <v>166</v>
       </c>
       <c r="N2">
         <v>1500</v>
@@ -1092,7 +1395,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1120,8 +1423,8 @@
       <c r="L3">
         <v>137589</v>
       </c>
-      <c r="M3">
-        <v>777273</v>
+      <c r="M3" t="s">
+        <v>167</v>
       </c>
       <c r="P3" t="s">
         <v>39</v>
@@ -1172,7 +1475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1200,8 +1503,8 @@
       <c r="L4">
         <v>126531</v>
       </c>
-      <c r="M4">
-        <v>296238</v>
+      <c r="M4" t="s">
+        <v>168</v>
       </c>
       <c r="P4" t="s">
         <v>39</v>
@@ -1252,7 +1555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1280,8 +1583,8 @@
       <c r="L5">
         <v>622144</v>
       </c>
-      <c r="M5">
-        <v>450834</v>
+      <c r="M5" t="s">
+        <v>169</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -1332,7 +1635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1360,8 +1663,8 @@
       <c r="L6">
         <v>991194</v>
       </c>
-      <c r="M6">
-        <v>873940</v>
+      <c r="M6" t="s">
+        <v>170</v>
       </c>
       <c r="P6" t="s">
         <v>39</v>
@@ -1412,7 +1715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1440,8 +1743,8 @@
       <c r="L7">
         <v>904392</v>
       </c>
-      <c r="M7">
-        <v>492134</v>
+      <c r="M7" t="s">
+        <v>171</v>
       </c>
       <c r="P7" t="s">
         <v>39</v>
@@ -1492,7 +1795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1520,8 +1823,8 @@
       <c r="L8">
         <v>834704</v>
       </c>
-      <c r="M8">
-        <v>972972</v>
+      <c r="M8" t="s">
+        <v>172</v>
       </c>
       <c r="P8" t="s">
         <v>39</v>
@@ -1572,7 +1875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1600,8 +1903,8 @@
       <c r="L9">
         <v>639564</v>
       </c>
-      <c r="M9">
-        <v>683741</v>
+      <c r="M9" t="s">
+        <v>173</v>
       </c>
       <c r="P9" t="s">
         <v>39</v>
@@ -1652,7 +1955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1680,8 +1983,8 @@
       <c r="L10">
         <v>759371</v>
       </c>
-      <c r="M10">
-        <v>599289</v>
+      <c r="M10" t="s">
+        <v>174</v>
       </c>
       <c r="P10" t="s">
         <v>39</v>
@@ -1732,7 +2035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1760,8 +2063,8 @@
       <c r="L11">
         <v>780470</v>
       </c>
-      <c r="M11">
-        <v>948121</v>
+      <c r="M11" t="s">
+        <v>175</v>
       </c>
       <c r="P11" t="s">
         <v>39</v>
@@ -1812,7 +2115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1840,8 +2143,8 @@
       <c r="L12">
         <v>431076</v>
       </c>
-      <c r="M12">
-        <v>795348</v>
+      <c r="M12" t="s">
+        <v>176</v>
       </c>
       <c r="P12" t="s">
         <v>39</v>
@@ -1892,7 +2195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1920,8 +2223,8 @@
       <c r="L13">
         <v>868362</v>
       </c>
-      <c r="M13">
-        <v>832866</v>
+      <c r="M13" t="s">
+        <v>177</v>
       </c>
       <c r="P13" t="s">
         <v>39</v>
@@ -1972,7 +2275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2000,8 +2303,8 @@
       <c r="L14">
         <v>460913</v>
       </c>
-      <c r="M14">
-        <v>424272</v>
+      <c r="M14" t="s">
+        <v>178</v>
       </c>
       <c r="P14" t="s">
         <v>39</v>
@@ -2052,7 +2355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2080,8 +2383,8 @@
       <c r="L15">
         <v>157671</v>
       </c>
-      <c r="M15">
-        <v>348830</v>
+      <c r="M15" t="s">
+        <v>179</v>
       </c>
       <c r="P15" t="s">
         <v>39</v>
@@ -2132,7 +2435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2160,8 +2463,8 @@
       <c r="L16">
         <v>937925</v>
       </c>
-      <c r="M16">
-        <v>735744</v>
+      <c r="M16" t="s">
+        <v>180</v>
       </c>
       <c r="P16" t="s">
         <v>39</v>
@@ -2212,7 +2515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2240,8 +2543,8 @@
       <c r="L17">
         <v>165921</v>
       </c>
-      <c r="M17">
-        <v>839595</v>
+      <c r="M17" t="s">
+        <v>181</v>
       </c>
       <c r="P17" t="s">
         <v>39</v>
@@ -2292,7 +2595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2320,8 +2623,8 @@
       <c r="L18">
         <v>807143</v>
       </c>
-      <c r="M18">
-        <v>574065</v>
+      <c r="M18" t="s">
+        <v>182</v>
       </c>
       <c r="P18" t="s">
         <v>39</v>
@@ -2372,7 +2675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2400,8 +2703,8 @@
       <c r="L19">
         <v>298867</v>
       </c>
-      <c r="M19">
-        <v>476320</v>
+      <c r="M19" t="s">
+        <v>183</v>
       </c>
       <c r="P19" t="s">
         <v>39</v>
@@ -2452,7 +2755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -2480,8 +2783,8 @@
       <c r="L20">
         <v>914284</v>
       </c>
-      <c r="M20">
-        <v>797616</v>
+      <c r="M20" t="s">
+        <v>184</v>
       </c>
       <c r="P20" t="s">
         <v>39</v>
@@ -2532,7 +2835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -2560,8 +2863,8 @@
       <c r="L21">
         <v>732516</v>
       </c>
-      <c r="M21">
-        <v>832280</v>
+      <c r="M21" t="s">
+        <v>185</v>
       </c>
       <c r="P21" t="s">
         <v>39</v>
@@ -2612,7 +2915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2640,8 +2943,8 @@
       <c r="L22">
         <v>235354</v>
       </c>
-      <c r="M22">
-        <v>744438</v>
+      <c r="M22" t="s">
+        <v>186</v>
       </c>
       <c r="P22" t="s">
         <v>39</v>
@@ -2692,7 +2995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -2720,8 +3023,8 @@
       <c r="L23">
         <v>983505</v>
       </c>
-      <c r="M23">
-        <v>913881</v>
+      <c r="M23" t="s">
+        <v>187</v>
       </c>
       <c r="P23" t="s">
         <v>39</v>
@@ -2772,7 +3075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2800,8 +3103,8 @@
       <c r="L24">
         <v>540246</v>
       </c>
-      <c r="M24">
-        <v>999154</v>
+      <c r="M24" t="s">
+        <v>188</v>
       </c>
       <c r="P24" t="s">
         <v>39</v>
@@ -2852,7 +3155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2880,8 +3183,8 @@
       <c r="L25">
         <v>669811</v>
       </c>
-      <c r="M25">
-        <v>393850</v>
+      <c r="M25" t="s">
+        <v>189</v>
       </c>
       <c r="P25" t="s">
         <v>39</v>
@@ -2932,7 +3235,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -2960,8 +3263,8 @@
       <c r="L26">
         <v>658136</v>
       </c>
-      <c r="M26">
-        <v>184803</v>
+      <c r="M26" t="s">
+        <v>190</v>
       </c>
       <c r="P26" t="s">
         <v>39</v>
@@ -3012,7 +3315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -3040,8 +3343,8 @@
       <c r="L27">
         <v>499011</v>
       </c>
-      <c r="M27">
-        <v>261668</v>
+      <c r="M27" t="s">
+        <v>191</v>
       </c>
       <c r="P27" t="s">
         <v>39</v>
@@ -3092,7 +3395,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3120,8 +3423,8 @@
       <c r="L28">
         <v>323266</v>
       </c>
-      <c r="M28">
-        <v>796468</v>
+      <c r="M28" t="s">
+        <v>192</v>
       </c>
       <c r="P28" t="s">
         <v>39</v>
@@ -3172,7 +3475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -3200,8 +3503,8 @@
       <c r="L29">
         <v>289675</v>
       </c>
-      <c r="M29">
-        <v>337211</v>
+      <c r="M29" t="s">
+        <v>193</v>
       </c>
       <c r="P29" t="s">
         <v>39</v>
@@ -3252,7 +3555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -3280,8 +3583,8 @@
       <c r="L30">
         <v>211183</v>
       </c>
-      <c r="M30">
-        <v>639411</v>
+      <c r="M30" t="s">
+        <v>194</v>
       </c>
       <c r="P30" t="s">
         <v>39</v>
@@ -3332,7 +3635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -3360,8 +3663,8 @@
       <c r="L31">
         <v>143391</v>
       </c>
-      <c r="M31">
-        <v>425682</v>
+      <c r="M31" t="s">
+        <v>195</v>
       </c>
       <c r="P31" t="s">
         <v>39</v>
@@ -3412,7 +3715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -3440,8 +3743,8 @@
       <c r="L32">
         <v>544501</v>
       </c>
-      <c r="M32">
-        <v>984509</v>
+      <c r="M32" t="s">
+        <v>196</v>
       </c>
       <c r="P32" t="s">
         <v>39</v>
@@ -3492,7 +3795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -3520,8 +3823,8 @@
       <c r="L33">
         <v>928437</v>
       </c>
-      <c r="M33">
-        <v>988482</v>
+      <c r="M33" t="s">
+        <v>197</v>
       </c>
       <c r="P33" t="s">
         <v>39</v>
@@ -3572,7 +3875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -3600,8 +3903,8 @@
       <c r="L34">
         <v>814726</v>
       </c>
-      <c r="M34">
-        <v>492484</v>
+      <c r="M34" t="s">
+        <v>198</v>
       </c>
       <c r="P34" t="s">
         <v>39</v>
@@ -3652,7 +3955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -3680,8 +3983,8 @@
       <c r="L35">
         <v>620327</v>
       </c>
-      <c r="M35">
-        <v>292826</v>
+      <c r="M35" t="s">
+        <v>199</v>
       </c>
       <c r="P35" t="s">
         <v>39</v>
@@ -3732,7 +4035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -3760,8 +4063,8 @@
       <c r="L36">
         <v>531986</v>
       </c>
-      <c r="M36">
-        <v>762523</v>
+      <c r="M36" t="s">
+        <v>200</v>
       </c>
       <c r="P36" t="s">
         <v>39</v>
@@ -3812,7 +4115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -3840,8 +4143,8 @@
       <c r="L37">
         <v>549585</v>
       </c>
-      <c r="M37">
-        <v>363385</v>
+      <c r="M37" t="s">
+        <v>201</v>
       </c>
       <c r="P37" t="s">
         <v>39</v>
@@ -3892,7 +4195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -3920,8 +4223,8 @@
       <c r="L38">
         <v>240236</v>
       </c>
-      <c r="M38">
-        <v>195043</v>
+      <c r="M38" t="s">
+        <v>202</v>
       </c>
       <c r="P38" t="s">
         <v>39</v>
@@ -3972,7 +4275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -4000,8 +4303,8 @@
       <c r="L39">
         <v>807684</v>
       </c>
-      <c r="M39">
-        <v>204430</v>
+      <c r="M39" t="s">
+        <v>203</v>
       </c>
       <c r="P39" t="s">
         <v>39</v>
@@ -4052,7 +4355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -4080,8 +4383,8 @@
       <c r="L40">
         <v>717709</v>
       </c>
-      <c r="M40">
-        <v>746329</v>
+      <c r="M40" t="s">
+        <v>204</v>
       </c>
       <c r="P40" t="s">
         <v>39</v>
@@ -4132,7 +4435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -4160,8 +4463,8 @@
       <c r="L41">
         <v>667004</v>
       </c>
-      <c r="M41">
-        <v>483650</v>
+      <c r="M41" t="s">
+        <v>205</v>
       </c>
       <c r="P41" t="s">
         <v>39</v>
@@ -4212,7 +4515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -4240,8 +4543,8 @@
       <c r="L42">
         <v>496275</v>
       </c>
-      <c r="M42">
-        <v>171403</v>
+      <c r="M42" t="s">
+        <v>206</v>
       </c>
       <c r="P42" t="s">
         <v>39</v>
@@ -4292,7 +4595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -4320,8 +4623,8 @@
       <c r="L43">
         <v>643700</v>
       </c>
-      <c r="M43">
-        <v>325379</v>
+      <c r="M43" t="s">
+        <v>207</v>
       </c>
       <c r="P43" t="s">
         <v>39</v>
@@ -4372,7 +4675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -4400,8 +4703,8 @@
       <c r="L44">
         <v>534985</v>
       </c>
-      <c r="M44">
-        <v>404568</v>
+      <c r="M44" t="s">
+        <v>208</v>
       </c>
       <c r="P44" t="s">
         <v>39</v>
@@ -4452,7 +4755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -4480,8 +4783,8 @@
       <c r="L45">
         <v>193486</v>
       </c>
-      <c r="M45">
-        <v>717970</v>
+      <c r="M45" t="s">
+        <v>209</v>
       </c>
       <c r="P45" t="s">
         <v>39</v>
@@ -4532,7 +4835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -4560,8 +4863,8 @@
       <c r="L46">
         <v>896584</v>
       </c>
-      <c r="M46">
-        <v>981394</v>
+      <c r="M46" t="s">
+        <v>210</v>
       </c>
       <c r="P46" t="s">
         <v>39</v>
@@ -4612,7 +4915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -4640,8 +4943,8 @@
       <c r="L47">
         <v>398997</v>
       </c>
-      <c r="M47">
-        <v>502118</v>
+      <c r="M47" t="s">
+        <v>211</v>
       </c>
       <c r="P47" t="s">
         <v>39</v>
@@ -4692,7 +4995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -4720,8 +5023,8 @@
       <c r="L48">
         <v>213016</v>
       </c>
-      <c r="M48">
-        <v>799978</v>
+      <c r="M48" t="s">
+        <v>212</v>
       </c>
       <c r="P48" t="s">
         <v>39</v>
@@ -4772,7 +5075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -4800,8 +5103,8 @@
       <c r="L49">
         <v>366146</v>
       </c>
-      <c r="M49">
-        <v>463003</v>
+      <c r="M49" t="s">
+        <v>213</v>
       </c>
       <c r="P49" t="s">
         <v>39</v>
@@ -4852,7 +5155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -4880,8 +5183,8 @@
       <c r="L50">
         <v>968614</v>
       </c>
-      <c r="M50">
-        <v>380451</v>
+      <c r="M50" t="s">
+        <v>214</v>
       </c>
       <c r="P50" t="s">
         <v>39</v>
@@ -4932,7 +5235,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -4960,8 +5263,8 @@
       <c r="L51">
         <v>320338</v>
       </c>
-      <c r="M51">
-        <v>749027</v>
+      <c r="M51" t="s">
+        <v>215</v>
       </c>
       <c r="P51" t="s">
         <v>39</v>
@@ -5012,7 +5315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -5040,8 +5343,8 @@
       <c r="L52">
         <v>477711</v>
       </c>
-      <c r="M52">
-        <v>366282</v>
+      <c r="M52" t="s">
+        <v>216</v>
       </c>
       <c r="P52" t="s">
         <v>39</v>
@@ -5092,7 +5395,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -5120,8 +5423,8 @@
       <c r="L53">
         <v>730422</v>
       </c>
-      <c r="M53">
-        <v>543968</v>
+      <c r="M53" t="s">
+        <v>217</v>
       </c>
       <c r="P53" t="s">
         <v>39</v>
@@ -5172,7 +5475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>96</v>
       </c>
@@ -5200,8 +5503,8 @@
       <c r="L54">
         <v>991517</v>
       </c>
-      <c r="M54">
-        <v>757673</v>
+      <c r="M54" t="s">
+        <v>218</v>
       </c>
       <c r="P54" t="s">
         <v>39</v>
@@ -5252,7 +5555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
@@ -5280,8 +5583,8 @@
       <c r="L55">
         <v>753426</v>
       </c>
-      <c r="M55">
-        <v>444532</v>
+      <c r="M55" t="s">
+        <v>219</v>
       </c>
       <c r="P55" t="s">
         <v>39</v>
@@ -5332,7 +5635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>98</v>
       </c>
@@ -5360,8 +5663,8 @@
       <c r="L56">
         <v>995419</v>
       </c>
-      <c r="M56">
-        <v>267798</v>
+      <c r="M56" t="s">
+        <v>220</v>
       </c>
       <c r="P56" t="s">
         <v>39</v>
@@ -5412,7 +5715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>99</v>
       </c>
@@ -5440,8 +5743,8 @@
       <c r="L57">
         <v>905546</v>
       </c>
-      <c r="M57">
-        <v>332164</v>
+      <c r="M57" t="s">
+        <v>221</v>
       </c>
       <c r="P57" t="s">
         <v>39</v>
@@ -5492,7 +5795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -5520,8 +5823,8 @@
       <c r="L58">
         <v>296921</v>
       </c>
-      <c r="M58">
-        <v>261019</v>
+      <c r="M58" t="s">
+        <v>222</v>
       </c>
       <c r="P58" t="s">
         <v>39</v>
@@ -5572,7 +5875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -5600,8 +5903,8 @@
       <c r="L59">
         <v>455891</v>
       </c>
-      <c r="M59">
-        <v>173084</v>
+      <c r="M59" t="s">
+        <v>223</v>
       </c>
       <c r="P59" t="s">
         <v>39</v>
@@ -5652,7 +5955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -5680,8 +5983,8 @@
       <c r="L60">
         <v>469335</v>
       </c>
-      <c r="M60">
-        <v>779409</v>
+      <c r="M60" t="s">
+        <v>224</v>
       </c>
       <c r="P60" t="s">
         <v>39</v>
@@ -5732,7 +6035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -5760,8 +6063,8 @@
       <c r="L61">
         <v>192884</v>
       </c>
-      <c r="M61">
-        <v>593351</v>
+      <c r="M61" t="s">
+        <v>225</v>
       </c>
       <c r="P61" t="s">
         <v>39</v>
@@ -5812,7 +6115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>104</v>
       </c>
@@ -5840,8 +6143,8 @@
       <c r="L62">
         <v>173466</v>
       </c>
-      <c r="M62">
-        <v>788727</v>
+      <c r="M62" t="s">
+        <v>226</v>
       </c>
       <c r="P62" t="s">
         <v>39</v>
@@ -5892,7 +6195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -5920,8 +6223,8 @@
       <c r="L63">
         <v>556943</v>
       </c>
-      <c r="M63">
-        <v>494212</v>
+      <c r="M63" t="s">
+        <v>227</v>
       </c>
       <c r="P63" t="s">
         <v>39</v>
@@ -5972,7 +6275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -6000,8 +6303,8 @@
       <c r="L64">
         <v>259185</v>
       </c>
-      <c r="M64">
-        <v>252865</v>
+      <c r="M64" t="s">
+        <v>228</v>
       </c>
       <c r="P64" t="s">
         <v>39</v>
@@ -6052,7 +6355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -6080,8 +6383,8 @@
       <c r="L65">
         <v>605554</v>
       </c>
-      <c r="M65">
-        <v>381110</v>
+      <c r="M65" t="s">
+        <v>229</v>
       </c>
       <c r="P65" t="s">
         <v>39</v>
@@ -6132,7 +6435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -6160,8 +6463,8 @@
       <c r="L66">
         <v>584617</v>
       </c>
-      <c r="M66">
-        <v>958434</v>
+      <c r="M66" t="s">
+        <v>230</v>
       </c>
       <c r="P66" t="s">
         <v>39</v>
@@ -6212,7 +6515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>109</v>
       </c>
@@ -6240,8 +6543,8 @@
       <c r="L67">
         <v>722822</v>
       </c>
-      <c r="M67">
-        <v>786256</v>
+      <c r="M67" t="s">
+        <v>231</v>
       </c>
       <c r="P67" t="s">
         <v>39</v>
@@ -6292,7 +6595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -6320,8 +6623,8 @@
       <c r="L68">
         <v>234661</v>
       </c>
-      <c r="M68">
-        <v>355320</v>
+      <c r="M68" t="s">
+        <v>232</v>
       </c>
       <c r="P68" t="s">
         <v>39</v>
@@ -6372,7 +6675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>111</v>
       </c>
@@ -6400,8 +6703,8 @@
       <c r="L69">
         <v>362978</v>
       </c>
-      <c r="M69">
-        <v>486219</v>
+      <c r="M69" t="s">
+        <v>233</v>
       </c>
       <c r="P69" t="s">
         <v>39</v>
@@ -6452,7 +6755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -6480,8 +6783,8 @@
       <c r="L70">
         <v>205267</v>
       </c>
-      <c r="M70">
-        <v>358863</v>
+      <c r="M70" t="s">
+        <v>234</v>
       </c>
       <c r="P70" t="s">
         <v>39</v>
@@ -6532,7 +6835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>113</v>
       </c>
@@ -6560,8 +6863,8 @@
       <c r="L71">
         <v>929732</v>
       </c>
-      <c r="M71">
-        <v>560814</v>
+      <c r="M71" t="s">
+        <v>235</v>
       </c>
       <c r="P71" t="s">
         <v>39</v>
@@ -6612,7 +6915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -6640,8 +6943,8 @@
       <c r="L72">
         <v>561901</v>
       </c>
-      <c r="M72">
-        <v>814488</v>
+      <c r="M72" t="s">
+        <v>236</v>
       </c>
       <c r="P72" t="s">
         <v>39</v>
@@ -6692,7 +6995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -6720,8 +7023,8 @@
       <c r="L73">
         <v>555642</v>
       </c>
-      <c r="M73">
-        <v>294187</v>
+      <c r="M73" t="s">
+        <v>237</v>
       </c>
       <c r="P73" t="s">
         <v>39</v>
@@ -6772,7 +7075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>116</v>
       </c>
@@ -6800,8 +7103,8 @@
       <c r="L74">
         <v>246175</v>
       </c>
-      <c r="M74">
-        <v>386877</v>
+      <c r="M74" t="s">
+        <v>238</v>
       </c>
       <c r="P74" t="s">
         <v>39</v>
@@ -6852,7 +7155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>117</v>
       </c>
@@ -6880,8 +7183,8 @@
       <c r="L75">
         <v>935519</v>
       </c>
-      <c r="M75">
-        <v>195111</v>
+      <c r="M75" t="s">
+        <v>239</v>
       </c>
       <c r="P75" t="s">
         <v>39</v>
@@ -6932,7 +7235,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -6960,8 +7263,8 @@
       <c r="L76">
         <v>100084</v>
       </c>
-      <c r="M76">
-        <v>773847</v>
+      <c r="M76" t="s">
+        <v>240</v>
       </c>
       <c r="P76" t="s">
         <v>39</v>
@@ -7012,7 +7315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -7040,8 +7343,8 @@
       <c r="L77">
         <v>795319</v>
       </c>
-      <c r="M77">
-        <v>268100</v>
+      <c r="M77" t="s">
+        <v>241</v>
       </c>
       <c r="P77" t="s">
         <v>39</v>
@@ -7092,7 +7395,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>120</v>
       </c>
@@ -7120,8 +7423,8 @@
       <c r="L78">
         <v>494047</v>
       </c>
-      <c r="M78">
-        <v>514300</v>
+      <c r="M78" t="s">
+        <v>242</v>
       </c>
       <c r="P78" t="s">
         <v>39</v>
@@ -7172,7 +7475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -7200,8 +7503,8 @@
       <c r="L79">
         <v>109593</v>
       </c>
-      <c r="M79">
-        <v>656189</v>
+      <c r="M79" t="s">
+        <v>243</v>
       </c>
       <c r="P79" t="s">
         <v>39</v>
@@ -7252,7 +7555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>122</v>
       </c>
@@ -7280,8 +7583,8 @@
       <c r="L80">
         <v>453672</v>
       </c>
-      <c r="M80">
-        <v>498604</v>
+      <c r="M80" t="s">
+        <v>244</v>
       </c>
       <c r="P80" t="s">
         <v>39</v>
@@ -7332,7 +7635,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>123</v>
       </c>
@@ -7360,8 +7663,8 @@
       <c r="L81">
         <v>539632</v>
       </c>
-      <c r="M81">
-        <v>450835</v>
+      <c r="M81" t="s">
+        <v>245</v>
       </c>
       <c r="P81" t="s">
         <v>39</v>
@@ -7412,7 +7715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>124</v>
       </c>
@@ -7440,8 +7743,8 @@
       <c r="L82">
         <v>168610</v>
       </c>
-      <c r="M82">
-        <v>511359</v>
+      <c r="M82" t="s">
+        <v>246</v>
       </c>
       <c r="P82" t="s">
         <v>39</v>
@@ -7492,7 +7795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>125</v>
       </c>
@@ -7520,8 +7823,8 @@
       <c r="L83">
         <v>935676</v>
       </c>
-      <c r="M83">
-        <v>524215</v>
+      <c r="M83" t="s">
+        <v>247</v>
       </c>
       <c r="P83" t="s">
         <v>39</v>
@@ -7572,7 +7875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>126</v>
       </c>
@@ -7600,8 +7903,8 @@
       <c r="L84">
         <v>124998</v>
       </c>
-      <c r="M84">
-        <v>631224</v>
+      <c r="M84" t="s">
+        <v>248</v>
       </c>
       <c r="P84" t="s">
         <v>39</v>
@@ -7652,7 +7955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>127</v>
       </c>
@@ -7680,8 +7983,8 @@
       <c r="L85">
         <v>956145</v>
       </c>
-      <c r="M85">
-        <v>944948</v>
+      <c r="M85" t="s">
+        <v>249</v>
       </c>
       <c r="P85" t="s">
         <v>39</v>
@@ -7732,7 +8035,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>128</v>
       </c>
@@ -7760,8 +8063,8 @@
       <c r="L86">
         <v>339213</v>
       </c>
-      <c r="M86">
-        <v>448438</v>
+      <c r="M86" t="s">
+        <v>250</v>
       </c>
       <c r="P86" t="s">
         <v>39</v>
@@ -7812,7 +8115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>129</v>
       </c>
@@ -7840,8 +8143,8 @@
       <c r="L87">
         <v>542170</v>
       </c>
-      <c r="M87">
-        <v>743491</v>
+      <c r="M87" t="s">
+        <v>251</v>
       </c>
       <c r="P87" t="s">
         <v>39</v>
@@ -7892,7 +8195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>130</v>
       </c>
@@ -7920,8 +8223,8 @@
       <c r="L88">
         <v>130047</v>
       </c>
-      <c r="M88">
-        <v>827371</v>
+      <c r="M88" t="s">
+        <v>252</v>
       </c>
       <c r="P88" t="s">
         <v>39</v>
@@ -7972,7 +8275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>131</v>
       </c>
@@ -8000,8 +8303,8 @@
       <c r="L89">
         <v>556062</v>
       </c>
-      <c r="M89">
-        <v>373517</v>
+      <c r="M89" t="s">
+        <v>253</v>
       </c>
       <c r="P89" t="s">
         <v>39</v>
@@ -8052,7 +8355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>132</v>
       </c>
@@ -8080,8 +8383,8 @@
       <c r="L90">
         <v>575065</v>
       </c>
-      <c r="M90">
-        <v>255342</v>
+      <c r="M90" t="s">
+        <v>254</v>
       </c>
       <c r="P90" t="s">
         <v>39</v>
@@ -8132,7 +8435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>133</v>
       </c>
@@ -8160,8 +8463,8 @@
       <c r="L91">
         <v>418697</v>
       </c>
-      <c r="M91">
-        <v>259333</v>
+      <c r="M91" t="s">
+        <v>255</v>
       </c>
       <c r="P91" t="s">
         <v>39</v>
@@ -8212,7 +8515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>134</v>
       </c>
@@ -8240,8 +8543,8 @@
       <c r="L92">
         <v>552312</v>
       </c>
-      <c r="M92">
-        <v>380089</v>
+      <c r="M92" t="s">
+        <v>256</v>
       </c>
       <c r="P92" t="s">
         <v>39</v>
@@ -8292,7 +8595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>135</v>
       </c>
@@ -8320,8 +8623,8 @@
       <c r="L93">
         <v>196567</v>
       </c>
-      <c r="M93">
-        <v>878252</v>
+      <c r="M93" t="s">
+        <v>257</v>
       </c>
       <c r="P93" t="s">
         <v>39</v>
@@ -8372,7 +8675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>136</v>
       </c>
@@ -8400,8 +8703,8 @@
       <c r="L94">
         <v>712462</v>
       </c>
-      <c r="M94">
-        <v>373686</v>
+      <c r="M94" t="s">
+        <v>258</v>
       </c>
       <c r="P94" t="s">
         <v>39</v>
@@ -8452,7 +8755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>137</v>
       </c>
@@ -8480,8 +8783,8 @@
       <c r="L95">
         <v>688262</v>
       </c>
-      <c r="M95">
-        <v>503010</v>
+      <c r="M95" t="s">
+        <v>259</v>
       </c>
       <c r="P95" t="s">
         <v>39</v>
@@ -8532,7 +8835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>138</v>
       </c>
@@ -8560,8 +8863,8 @@
       <c r="L96">
         <v>978611</v>
       </c>
-      <c r="M96">
-        <v>312888</v>
+      <c r="M96" t="s">
+        <v>260</v>
       </c>
       <c r="P96" t="s">
         <v>39</v>
@@ -8612,7 +8915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>139</v>
       </c>
@@ -8640,8 +8943,8 @@
       <c r="L97">
         <v>586576</v>
       </c>
-      <c r="M97">
-        <v>123989</v>
+      <c r="M97" t="s">
+        <v>261</v>
       </c>
       <c r="P97" t="s">
         <v>39</v>
@@ -8692,7 +8995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>140</v>
       </c>
@@ -8720,8 +9023,8 @@
       <c r="L98">
         <v>907179</v>
       </c>
-      <c r="M98">
-        <v>673848</v>
+      <c r="M98" t="s">
+        <v>262</v>
       </c>
       <c r="P98" t="s">
         <v>39</v>
@@ -8772,7 +9075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>141</v>
       </c>
@@ -8800,8 +9103,8 @@
       <c r="L99">
         <v>146926</v>
       </c>
-      <c r="M99">
-        <v>401558</v>
+      <c r="M99" t="s">
+        <v>263</v>
       </c>
       <c r="P99" t="s">
         <v>39</v>
@@ -8852,7 +9155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>142</v>
       </c>
@@ -8880,8 +9183,8 @@
       <c r="L100">
         <v>564310</v>
       </c>
-      <c r="M100">
-        <v>115401</v>
+      <c r="M100" t="s">
+        <v>264</v>
       </c>
       <c r="P100" t="s">
         <v>39</v>
@@ -8932,7 +9235,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>143</v>
       </c>
@@ -8960,8 +9263,8 @@
       <c r="L101">
         <v>827355</v>
       </c>
-      <c r="M101">
-        <v>941224</v>
+      <c r="M101" t="s">
+        <v>265</v>
       </c>
       <c r="P101" t="s">
         <v>39</v>
@@ -9012,7 +9315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>144</v>
       </c>
@@ -9040,8 +9343,8 @@
       <c r="L102">
         <v>376548</v>
       </c>
-      <c r="M102">
-        <v>575799</v>
+      <c r="M102" t="s">
+        <v>266</v>
       </c>
       <c r="P102" t="s">
         <v>39</v>

</xml_diff>